<commit_message>
New data for iotamotion testing. Also lots of updated generated output files
</commit_message>
<xml_diff>
--- a/output_file/October Y=0/example.xlsx
+++ b/output_file/October Y=0/example.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>MetalShape</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Validity_Check_Value_of_Rotation_Error</t>
+  </si>
+  <si>
+    <t>Copper</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -440,13 +443,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>4.3368086899420177E-19</v>
+        <v>2.7756422635651865E-17</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -457,13 +460,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>1.788112030672749E-18</v>
+        <v>4.3368086899420177E-19</v>
       </c>
       <c r="D6">
-        <v>3.8362336943035803E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -471,13 +474,41 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1.788112030672749E-18</v>
+      </c>
+      <c r="D7">
+        <v>3.8362336943035803E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>1.1162030000000153E-4</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>5.4230322089694619E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>2.7756422635651865E-17</v>
+      </c>
+      <c r="D9">
+        <v>3.8397243338001336E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>